<commit_message>
Settings on Gameplay Abilities
1. Excel 分頁有註記

Gameplay Tag 描述
Ability Tags 此能力具有以下標籤
Cancel Abilities with Tag 具有這些標籤的能力會被執行
Block Abilities with Tag 在此能力活躍時，具有這些標籤的能力會被阻擋
Activation Owned Tags 啟動擁有標籤在此能力啟動時應用於啟動擁有者的標籤
Replicated Tags 如果在AbilitySystemGlobals中啟用了ReplicateActivationOwnedTags
Activation Required Tags 只有激活角色/組件具有所有這些標籤才能啟動此能力
Activation Blocked Tags 如果激活角色/組件具有任何這些標籤，則此能力被阻擋
Source Required Tags 只有來源角色/組件具有所有這些標籤才能啟動此能力
Source Blocked Tags 如果來源角色/組件具有任何這些標籤，則此能力被阻擋
Target Required Tags 只有目標角色/組件具有所有這些標籤才能啟動此能力
Target Blocked Tags 如果目標角色/組件具有任何這些標籤，則此能力被阻擋

政策類型 描述 細節
Instanced Per Actor 為每個技能創建單個實例，每次啟動時重複使用 可以存儲持久數據。每次都必須手動重置變量。
Instanced Per Execution 每次啟動時都創建新的實例 不會在啟動之間存儲持久數據。比每個角色實例化稍差效能。
Non-Instanced 僅使用類默認對象，不創建實例 不能存儲狀態，不能綁定到能力任務的代理。是三個選項中效能最佳的。

不應使用的事項：

複製政策：無用。請勿使用。請參考Epic的能力系統問題，以瞭解Epic的解釋。遊戲玩法能力已經從伺服器複製到擁有的客戶端。
注意：遊戲玩法能力不運行於模擬代理（請使用GEs和GCs）。
伺服器尊重遠程能力取消：當本地客戶端的能力結束時，伺服器的能力也會結束。通常不是一個好主意；重要的是伺服器的版本。
直接複製輸入：總是將輸入按壓/釋放事件直接複製到伺服器。Epic不鼓勵這樣做。
</commit_message>
<xml_diff>
--- a/屬性設計.xlsx
+++ b/屬性設計.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UnrealProject\GIT\Aura_UE_Version_5_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD10D72-D7E5-49C8-BF18-1576468A14AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AB20D2-7AA2-4324-BA22-F859111DAC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="240" windowWidth="28800" windowHeight="15345" xr2:uid="{AE4780B8-E891-45A1-894A-4419F0287300}"/>
+    <workbookView xWindow="-360" yWindow="4335" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{AE4780B8-E891-45A1-894A-4419F0287300}"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="屬性基礎" sheetId="1" r:id="rId1"/>
+    <sheet name="注意事項" sheetId="4" r:id="rId2"/>
+    <sheet name="Instancing Policy" sheetId="2" r:id="rId3"/>
+    <sheet name="Tags" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
   <si>
     <t>Block Chance</t>
   </si>
@@ -105,6 +108,212 @@
   </si>
   <si>
     <t>Max Health</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instanced Per Actor</t>
+  </si>
+  <si>
+    <t>Instanced Per Execution</t>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A single instance is created for the ability. It is reused with each activation.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New instance created witheach activation</t>
+  </si>
+  <si>
+    <t>Non-Instanced</t>
+  </si>
+  <si>
+    <t>Only the Class Default Object is used, no instances are created.</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Can store persistent data.Variables must be manually reset each time.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Does not store persistent data between activations. Less performant than Instanced per Actor</t>
+  </si>
+  <si>
+    <t>Cannot store state, cannot bind to delegates on Ability Tasks. Best performance of the three options.</t>
+  </si>
+  <si>
+    <t>政策類型</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
+    <t>細節</t>
+  </si>
+  <si>
+    <t>為每個技能創建單個實例，每次啟動時重複使用</t>
+  </si>
+  <si>
+    <t>可以存儲持久數據。每次都必須手動重置變量。</t>
+  </si>
+  <si>
+    <t>每次啟動時都創建新的實例</t>
+  </si>
+  <si>
+    <t>不會在啟動之間存儲持久數據。比每個角色實例化稍差效能。</t>
+  </si>
+  <si>
+    <t>僅使用類默認對象，不創建實例</t>
+  </si>
+  <si>
+    <t>不能存儲狀態，不能綁定到能力任務的代理。是三個選項中效能最佳的。</t>
+  </si>
+  <si>
+    <t>Instancing Policy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gameplay Tag</t>
+  </si>
+  <si>
+    <t>此能力具有以下標籤</t>
+  </si>
+  <si>
+    <t>具有這些標籤的能力會被執行</t>
+  </si>
+  <si>
+    <t>Block Abilities with Tag</t>
+  </si>
+  <si>
+    <t>在此能力活躍時，具有這些標籤的能力會被阻擋</t>
+  </si>
+  <si>
+    <t>Activation Owned Tags</t>
+  </si>
+  <si>
+    <t>Replicated Tags</t>
+  </si>
+  <si>
+    <t>如果在AbilitySystemGlobals中啟用了ReplicateActivationOwnedTags</t>
+  </si>
+  <si>
+    <t>Activation Required Tags</t>
+  </si>
+  <si>
+    <t>只有激活角色/組件具有所有這些標籤才能啟動此能力</t>
+  </si>
+  <si>
+    <t>Activation Blocked Tags</t>
+  </si>
+  <si>
+    <t>如果激活角色/組件具有任何這些標籤，則此能力被阻擋</t>
+  </si>
+  <si>
+    <t>Source Required Tags</t>
+  </si>
+  <si>
+    <t>只有來源角色/組件具有所有這些標籤才能啟動此能力</t>
+  </si>
+  <si>
+    <t>Source Blocked Tags</t>
+  </si>
+  <si>
+    <t>如果來源角色/組件具有任何這些標籤，則此能力被阻擋</t>
+  </si>
+  <si>
+    <t>Target Required Tags</t>
+  </si>
+  <si>
+    <t>只有目標角色/組件具有所有這些標籤才能啟動此能力</t>
+  </si>
+  <si>
+    <t>Target Blocked Tags</t>
+  </si>
+  <si>
+    <t>如果目標角色/組件具有任何這些標籤，則此能力被阻擋</t>
+  </si>
+  <si>
+    <t>Ability Tags</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cancel Abilities with Tag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>啟動擁有標籤，在此能力啟動時應用於啟動擁有者的標籤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不應使用的事項：</t>
+  </si>
+  <si>
+    <t>注意：遊戲玩法能力不運行於模擬代理（請使用GEs和GCs）。</t>
+  </si>
+  <si>
+    <t>伺服器尊重遠程能力取消：當本地客戶端的能力結束時，伺服器的能力也會結束。通常不是一個好主意；重要的是伺服器的版本。</t>
+  </si>
+  <si>
+    <t>直接複製輸入：總是將輸入按壓/釋放事件直接複製到伺服器。Epic不鼓勵這樣做。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>複製政策：無用。請勿使用。請參考</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Epic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>的能力系統問題，以瞭解</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>Epic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="MS Gothic"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>的解釋。遊戲玩法能力已經從伺服器複製到擁有的客</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Malgun Gothic"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>戶端。</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -112,7 +321,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,8 +337,68 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF000000"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FF000000"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="MS Gothic"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Malgun Gothic"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Segoe UI"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,13 +423,62 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE3E3E3"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFE3E3E3"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE3E3E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE3E3E3"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFE3E3E3"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFE3E3E3"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE3E3E3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -169,7 +487,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -181,6 +499,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -197,6 +548,153 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9240534</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>639</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="圖片 1" descr="一張含有 文字, 螢幕擷取畫面, 軟體, 字型 的圖片&#10;&#10;自動產生的描述">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1C21D30-5DDE-CA77-F197-90BA9BCA5565}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="1752600"/>
+          <a:ext cx="9202434" cy="4582164"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>26640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3505201</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>105800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="圖片 1" descr="一張含有 文字, 螢幕擷取畫面, 字型 的圖片&#10;&#10;自動產生的描述">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4ED830A-CD67-A4B8-B54C-24DDB3163035}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66676" y="2198340"/>
+          <a:ext cx="10058400" cy="5527460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>458946</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>96328</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="圖片 1" descr="一張含有 文字, 螢幕擷取畫面, 字型, 數字 的圖片&#10;&#10;自動產生的描述">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13375629-64D3-4B5D-0DED-20029EDA8F4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3914775"/>
+          <a:ext cx="12508071" cy="7725853"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -518,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF685A25-C966-43CD-890A-4444B124481B}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -865,4 +1363,282 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5992FAC-6C36-4895-B477-02C6D324E583}">
+  <dimension ref="B2:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="10"/>
+    <col min="2" max="2" width="129" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE9A7DD-6CD8-47FF-A120-AAA417CC56C8}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B18:B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF11DD65-6FC3-4C19-AD24-272FF85F3A04}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>